<commit_message>
notebook 2 update FIXED BUG
</commit_message>
<xml_diff>
--- a/data/Path2/Path2-Model Training/UpdatedData.xlsx
+++ b/data/Path2/Path2-Model Training/UpdatedData.xlsx
@@ -420,10 +420,10 @@
         <v>0.8800000000000001</v>
       </c>
       <c r="D2">
-        <v>15.8564</v>
+        <v>15.91303</v>
       </c>
       <c r="E2">
-        <v>0.596736</v>
+        <v>0.5988671999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -437,10 +437,10 @@
         <v>0.76</v>
       </c>
       <c r="D3">
-        <v>16.815232</v>
+        <v>16.8752864</v>
       </c>
       <c r="E3">
-        <v>0.641648</v>
+        <v>0.6439395999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -454,10 +454,10 @@
         <v>0.8800000000000001</v>
       </c>
       <c r="D4">
-        <v>12.54008</v>
+        <v>12.584866</v>
       </c>
       <c r="E4">
-        <v>0.526624</v>
+        <v>0.5285048</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -471,10 +471,10 @@
         <v>0.9199999999999999</v>
       </c>
       <c r="D5">
-        <v>16.510928</v>
+        <v>16.5698956</v>
       </c>
       <c r="E5">
-        <v>0.595952</v>
+        <v>0.5980804</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -488,10 +488,10 @@
         <v>0.6800000000000002</v>
       </c>
       <c r="D6">
-        <v>17.6624</v>
+        <v>17.72548</v>
       </c>
       <c r="E6">
-        <v>0.466704</v>
+        <v>0.4683708</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -505,10 +505,10 @@
         <v>0.8</v>
       </c>
       <c r="D7">
-        <v>15.457008</v>
+        <v>15.5122116</v>
       </c>
       <c r="E7">
-        <v>0.6496</v>
+        <v>0.6519199999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -522,10 +522,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>14.188944</v>
+        <v>14.2396188</v>
       </c>
       <c r="E8">
-        <v>0.75208</v>
+        <v>0.7547659999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -539,10 +539,10 @@
         <v>1.4</v>
       </c>
       <c r="D9">
-        <v>13.33416</v>
+        <v>13.381782</v>
       </c>
       <c r="E9">
-        <v>1.31376</v>
+        <v>1.318452</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -556,10 +556,10 @@
         <v>0.3599999999999999</v>
       </c>
       <c r="D10">
-        <v>14.68488</v>
+        <v>14.737326</v>
       </c>
       <c r="E10">
-        <v>0.293552</v>
+        <v>0.2946004</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -573,10 +573,10 @@
         <v>0.6800000000000002</v>
       </c>
       <c r="D11">
-        <v>12.467728</v>
+        <v>12.5122556</v>
       </c>
       <c r="E11">
-        <v>0.6272</v>
+        <v>0.62944</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -590,10 +590,10 @@
         <v>0.4400000000000002</v>
       </c>
       <c r="D12">
-        <v>13.912192</v>
+        <v>13.9618784</v>
       </c>
       <c r="E12">
-        <v>0.348768</v>
+        <v>0.3500136</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -607,10 +607,10 @@
         <v>1.2</v>
       </c>
       <c r="D13">
-        <v>13.831776</v>
+        <v>13.8811752</v>
       </c>
       <c r="E13">
-        <v>0.884464</v>
+        <v>0.8876227999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -624,10 +624,10 @@
         <v>0.4800000000000002</v>
       </c>
       <c r="D14">
-        <v>14.059472</v>
+        <v>14.1096844</v>
       </c>
       <c r="E14">
-        <v>0.490896</v>
+        <v>0.4926492</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -641,10 +641,10 @@
         <v>0.6800000000000002</v>
       </c>
       <c r="D15">
-        <v>13.868848</v>
+        <v>13.9183796</v>
       </c>
       <c r="E15">
-        <v>0.616224</v>
+        <v>0.6184248</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -658,10 +658,10 @@
         <v>0.6400000000000001</v>
       </c>
       <c r="D16">
-        <v>13.041392</v>
+        <v>13.0879684</v>
       </c>
       <c r="E16">
-        <v>0.715792</v>
+        <v>0.7183484</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -675,10 +675,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D17">
-        <v>15.839264</v>
+        <v>15.8958328</v>
       </c>
       <c r="E17">
-        <v>0.564144</v>
+        <v>0.5661588</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -692,10 +692,10 @@
         <v>0.72</v>
       </c>
       <c r="D18">
-        <v>17.154592</v>
+        <v>17.2158584</v>
       </c>
       <c r="E18">
-        <v>0.553952</v>
+        <v>0.5559303999999999</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -709,10 +709,10 @@
         <v>0.6400000000000001</v>
       </c>
       <c r="D19">
-        <v>17.486112</v>
+        <v>17.5485624</v>
       </c>
       <c r="E19">
-        <v>0.5602239999999999</v>
+        <v>0.5622248</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -726,10 +726,10 @@
         <v>0.8800000000000001</v>
       </c>
       <c r="D20">
-        <v>12.59832</v>
+        <v>12.643314</v>
       </c>
       <c r="E20">
-        <v>0.755664</v>
+        <v>0.7583628</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -743,10 +743,10 @@
         <v>0.72</v>
       </c>
       <c r="D21">
-        <v>15.08192</v>
+        <v>15.135784</v>
       </c>
       <c r="E21">
-        <v>0.679392</v>
+        <v>0.6818183999999999</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -760,10 +760,10 @@
         <v>0.6400000000000001</v>
       </c>
       <c r="D22">
-        <v>15.489264</v>
+        <v>15.5445828</v>
       </c>
       <c r="E22">
-        <v>0.63336</v>
+        <v>0.635622</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -777,10 +777,10 @@
         <v>0.8399999999999999</v>
       </c>
       <c r="D23">
-        <v>15.534064</v>
+        <v>15.5895428</v>
       </c>
       <c r="E23">
-        <v>0.737632</v>
+        <v>0.7402664</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -794,10 +794,10 @@
         <v>0.8399999999999999</v>
       </c>
       <c r="D24">
-        <v>14.913024</v>
+        <v>14.9662848</v>
       </c>
       <c r="E24">
-        <v>0.681856</v>
+        <v>0.6842912</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -811,10 +811,10 @@
         <v>0.3599999999999999</v>
       </c>
       <c r="D25">
-        <v>14.328496</v>
+        <v>14.3796692</v>
       </c>
       <c r="E25">
-        <v>0.330736</v>
+        <v>0.3319172</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -828,10 +828,10 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="D26">
-        <v>12.552848</v>
+        <v>12.5976796</v>
       </c>
       <c r="E26">
-        <v>0.653072</v>
+        <v>0.6554044</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -845,10 +845,10 @@
         <v>1.28</v>
       </c>
       <c r="D27">
-        <v>13.79392</v>
+        <v>13.843184</v>
       </c>
       <c r="E27">
-        <v>1.35576</v>
+        <v>1.360602</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -862,10 +862,10 @@
         <v>0.52</v>
       </c>
       <c r="D28">
-        <v>12.912928</v>
+        <v>12.9590456</v>
       </c>
       <c r="E28">
-        <v>0.403312</v>
+        <v>0.4047524</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -879,10 +879,10 @@
         <v>0.4800000000000002</v>
       </c>
       <c r="D29">
-        <v>14.857024</v>
+        <v>14.9100848</v>
       </c>
       <c r="E29">
-        <v>0.473648</v>
+        <v>0.4753396</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -896,10 +896,10 @@
         <v>0.3199999999999998</v>
       </c>
       <c r="D30">
-        <v>15.397872</v>
+        <v>15.4528644</v>
       </c>
       <c r="E30">
-        <v>0.344624</v>
+        <v>0.3458548</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -913,10 +913,10 @@
         <v>0.24</v>
       </c>
       <c r="D31">
-        <v>18.53488</v>
+        <v>18.601076</v>
       </c>
       <c r="E31">
-        <v>0.235088</v>
+        <v>0.2359276</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -930,10 +930,10 @@
         <v>0.52</v>
       </c>
       <c r="D32">
-        <v>14.783776</v>
+        <v>14.8365752</v>
       </c>
       <c r="E32">
-        <v>0.476</v>
+        <v>0.4777</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -947,10 +947,10 @@
         <v>0.2</v>
       </c>
       <c r="D33">
-        <v>17.839248</v>
+        <v>17.9029596</v>
       </c>
       <c r="E33">
-        <v>0.31808</v>
+        <v>0.319216</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -964,10 +964,10 @@
         <v>0.4800000000000002</v>
       </c>
       <c r="D34">
-        <v>14.150304</v>
+        <v>14.2008408</v>
       </c>
       <c r="E34">
-        <v>0.676144</v>
+        <v>0.6785588</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -981,10 +981,10 @@
         <v>0.3599999999999999</v>
       </c>
       <c r="D35">
-        <v>17.1164</v>
+        <v>17.17753</v>
       </c>
       <c r="E35">
-        <v>0.391664</v>
+        <v>0.3930628</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -998,10 +998,10 @@
         <v>0.28</v>
       </c>
       <c r="D36">
-        <v>13.632752</v>
+        <v>13.6814404</v>
       </c>
       <c r="E36">
-        <v>0.356944</v>
+        <v>0.3582188</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1015,10 +1015,10 @@
         <v>0.4000000000000001</v>
       </c>
       <c r="D37">
-        <v>14.785232</v>
+        <v>14.8380364</v>
       </c>
       <c r="E37">
-        <v>0.469952</v>
+        <v>0.4716303999999999</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1032,10 +1032,10 @@
         <v>0.28</v>
       </c>
       <c r="D38">
-        <v>18.677568</v>
+        <v>18.7442736</v>
       </c>
       <c r="E38">
-        <v>0.262976</v>
+        <v>0.2639152</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1049,10 +1049,10 @@
         <v>0.4000000000000001</v>
       </c>
       <c r="D39">
-        <v>16.326688</v>
+        <v>16.3849976</v>
       </c>
       <c r="E39">
-        <v>0.515536</v>
+        <v>0.5173772</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1066,10 +1066,10 @@
         <v>0.4800000000000002</v>
       </c>
       <c r="D40">
-        <v>14.984928</v>
+        <v>15.0384456</v>
       </c>
       <c r="E40">
-        <v>0.502208</v>
+        <v>0.5040015999999999</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1083,10 +1083,10 @@
         <v>0.4400000000000002</v>
       </c>
       <c r="D41">
-        <v>14.578592</v>
+        <v>14.6306584</v>
       </c>
       <c r="E41">
-        <v>0.501872</v>
+        <v>0.5036644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>